<commit_message>
time to embark on these sync classes
</commit_message>
<xml_diff>
--- a/tests/Unit-AssetsMetadata-template20240209_tests.xlsx
+++ b/tests/Unit-AssetsMetadata-template20240209_tests.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="278">
   <si>
     <t xml:space="preserve"> ""</t>
   </si>
@@ -364,6 +364,12 @@
   </si>
   <si>
     <t xml:space="preserve">NMAI_019_33901000000018_p_01.mkv; NMAI_019_33901000000018_p_02.mkv; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CFCH Video Lab </t>
+  </si>
+  <si>
+    <t>AAA AV Transfer Lab</t>
   </si>
   <si>
     <t>Physical Format</t>
@@ -1730,11 +1736,11 @@
       <c r="E5" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>78</v>
+      <c r="F5" s="18" t="s">
+        <v>93</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>78</v>
+      <c r="G5" s="18" t="s">
+        <v>94</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>79</v>
@@ -38636,10 +38642,10 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="23" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
@@ -38668,442 +38674,442 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="24" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="24" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B3" s="24" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" ht="15.75" customHeight="1">
+      <c r="A4" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="24" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
-      <c r="A4" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="B4" s="24" t="s">
-        <v>96</v>
-      </c>
-    </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="24" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="24" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="24" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="24" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="24" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="24" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="24" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="24" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="24" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="24" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="24" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B16" s="24" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="24" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="24" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="24" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="24" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="24" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="24" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="24" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="24" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="24" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="24" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B26" s="24" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="24" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B27" s="24" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="28" ht="15.75" customHeight="1">
+      <c r="A28" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="B28" s="24" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="29" ht="15.75" customHeight="1">
+      <c r="A29" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="B29" s="24" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="30" ht="15.75" customHeight="1">
+      <c r="A30" s="24" t="s">
+        <v>149</v>
+      </c>
+      <c r="B30" s="24" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="31" ht="15.75" customHeight="1">
+      <c r="A31" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="B31" s="24" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="32" ht="15.75" customHeight="1">
+      <c r="A32" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="B32" s="24" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="33" ht="15.75" customHeight="1">
+      <c r="A33" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="B33" s="24" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="34" ht="15.75" customHeight="1">
+      <c r="A34" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="B34" s="24" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="35" ht="15.75" customHeight="1">
+      <c r="A35" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="B35" s="24" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="36" ht="15.75" customHeight="1">
+      <c r="A36" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="B36" s="24" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="37" ht="15.75" customHeight="1">
+      <c r="A37" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="B37" s="24" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="38" ht="15.75" customHeight="1">
+      <c r="A38" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="B38" s="24" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="39" ht="15.75" customHeight="1">
+      <c r="A39" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="B39" s="24" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="40" ht="15.75" customHeight="1">
+      <c r="A40" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="B40" s="24" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="41" ht="15.75" customHeight="1">
+      <c r="A41" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="B41" s="24" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="42" ht="15.75" customHeight="1">
+      <c r="A42" s="24" t="s">
+        <v>171</v>
+      </c>
+      <c r="B42" s="24" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="43" ht="15.75" customHeight="1">
+      <c r="A43" s="24" t="s">
+        <v>173</v>
+      </c>
+      <c r="B43" s="24" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="44" ht="15.75" customHeight="1">
+      <c r="A44" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="B44" s="24" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="45" ht="15.75" customHeight="1">
+      <c r="A45" s="24" t="s">
+        <v>177</v>
+      </c>
+      <c r="B45" s="24" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="46" ht="15.75" customHeight="1">
+      <c r="A46" s="24" t="s">
+        <v>179</v>
+      </c>
+      <c r="B46" s="24" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="47" ht="15.75" customHeight="1">
+      <c r="A47" s="24" t="s">
+        <v>181</v>
+      </c>
+      <c r="B47" s="24" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="48" ht="15.75" customHeight="1">
+      <c r="A48" s="24" t="s">
+        <v>183</v>
+      </c>
+      <c r="B48" s="24" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="49" ht="15.75" customHeight="1">
+      <c r="A49" s="24" t="s">
+        <v>185</v>
+      </c>
+      <c r="B49" s="24" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="50" ht="15.75" customHeight="1">
+      <c r="A50" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="B50" s="24" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="51" ht="15.75" customHeight="1">
+      <c r="A51" s="24" t="s">
+        <v>189</v>
+      </c>
+      <c r="B51" s="24" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="52" ht="15.75" customHeight="1">
+      <c r="A52" s="24" t="s">
+        <v>191</v>
+      </c>
+      <c r="B52" s="24" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="53" ht="15.75" customHeight="1">
+      <c r="A53" s="24" t="s">
+        <v>193</v>
+      </c>
+      <c r="B53" s="24" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="54" ht="15.75" customHeight="1">
+      <c r="A54" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="B54" s="24" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="55" ht="15.75" customHeight="1">
+      <c r="A55" s="24" t="s">
+        <v>197</v>
+      </c>
+      <c r="B55" s="24" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="24" t="s">
-        <v>144</v>
-      </c>
-      <c r="B28" s="24" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="24" t="s">
-        <v>145</v>
-      </c>
-      <c r="B29" s="24" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="24" t="s">
-        <v>147</v>
-      </c>
-      <c r="B30" s="24" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="24" t="s">
-        <v>149</v>
-      </c>
-      <c r="B31" s="24" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="24" t="s">
-        <v>150</v>
-      </c>
-      <c r="B32" s="24" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="24" t="s">
-        <v>152</v>
-      </c>
-      <c r="B33" s="24" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="24" t="s">
-        <v>154</v>
-      </c>
-      <c r="B34" s="24" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="24" t="s">
-        <v>156</v>
-      </c>
-      <c r="B35" s="24" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="24" t="s">
-        <v>158</v>
-      </c>
-      <c r="B36" s="24" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="24" t="s">
-        <v>160</v>
-      </c>
-      <c r="B37" s="24" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="24" t="s">
-        <v>162</v>
-      </c>
-      <c r="B38" s="24" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="24" t="s">
-        <v>164</v>
-      </c>
-      <c r="B39" s="24" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="24" t="s">
-        <v>166</v>
-      </c>
-      <c r="B40" s="24" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="24" t="s">
-        <v>167</v>
-      </c>
-      <c r="B41" s="24" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="24" t="s">
-        <v>169</v>
-      </c>
-      <c r="B42" s="24" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="24" t="s">
-        <v>171</v>
-      </c>
-      <c r="B43" s="24" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="24" t="s">
-        <v>173</v>
-      </c>
-      <c r="B44" s="24" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="24" t="s">
-        <v>175</v>
-      </c>
-      <c r="B45" s="24" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="24" t="s">
-        <v>177</v>
-      </c>
-      <c r="B46" s="24" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="24" t="s">
-        <v>179</v>
-      </c>
-      <c r="B47" s="24" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="24" t="s">
-        <v>181</v>
-      </c>
-      <c r="B48" s="24" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="24" t="s">
-        <v>183</v>
-      </c>
-      <c r="B49" s="24" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="24" t="s">
-        <v>185</v>
-      </c>
-      <c r="B50" s="24" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="24" t="s">
-        <v>187</v>
-      </c>
-      <c r="B51" s="24" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="24" t="s">
-        <v>189</v>
-      </c>
-      <c r="B52" s="24" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="24" t="s">
-        <v>191</v>
-      </c>
-      <c r="B53" s="24" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="24" t="s">
-        <v>193</v>
-      </c>
-      <c r="B54" s="24" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="24" t="s">
-        <v>195</v>
-      </c>
-      <c r="B55" s="24" t="s">
-        <v>141</v>
-      </c>
-    </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" s="24" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B56" s="24" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="57" ht="15.75" customHeight="1">
@@ -39111,439 +39117,439 @@
         <v>77</v>
       </c>
       <c r="B57" s="24" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="24" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B58" s="24" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="24" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B59" s="24" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="24" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B60" s="24" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="24" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B61" s="24" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="62" ht="15.75" customHeight="1">
       <c r="A62" s="24" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B62" s="24" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="24" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B63" s="24" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="A64" s="24" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B64" s="24" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="65" ht="15.75" customHeight="1">
       <c r="A65" s="24" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B65" s="24" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="24" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B66" s="24" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="67" ht="15.75" customHeight="1">
       <c r="A67" s="24" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B67" s="24" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="68" ht="15.75" customHeight="1">
       <c r="A68" s="24" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B68" s="24" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="69" ht="15.75" customHeight="1">
       <c r="A69" s="24" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B69" s="24" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="70" ht="15.75" customHeight="1">
       <c r="A70" s="24" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B70" s="24" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="71" ht="15.75" customHeight="1">
       <c r="A71" s="24" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B71" s="24" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="72" ht="15.75" customHeight="1">
+      <c r="A72" s="24" t="s">
+        <v>228</v>
+      </c>
+      <c r="B72" s="24" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="72" ht="15.75" customHeight="1">
-      <c r="A72" s="24" t="s">
-        <v>226</v>
-      </c>
-      <c r="B72" s="24" t="s">
-        <v>223</v>
-      </c>
-    </row>
     <row r="73" ht="15.75" customHeight="1">
       <c r="A73" s="24" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B73" s="24" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="74" ht="15.75" customHeight="1">
       <c r="A74" s="24" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B74" s="24" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="75" ht="15.75" customHeight="1">
       <c r="A75" s="24" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B75" s="24" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="76" ht="15.75" customHeight="1">
       <c r="A76" s="24" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B76" s="24" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="77" ht="15.75" customHeight="1">
+      <c r="A77" s="24" t="s">
+        <v>237</v>
+      </c>
+      <c r="B77" s="24" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="78" ht="15.75" customHeight="1">
+      <c r="A78" s="24" t="s">
+        <v>239</v>
+      </c>
+      <c r="B78" s="24" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="79" ht="15.75" customHeight="1">
+      <c r="A79" s="24" t="s">
+        <v>241</v>
+      </c>
+      <c r="B79" s="24" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="80" ht="15.75" customHeight="1">
+      <c r="A80" s="24" t="s">
+        <v>242</v>
+      </c>
+      <c r="B80" s="24" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="81" ht="15.75" customHeight="1">
+      <c r="A81" s="24" t="s">
+        <v>244</v>
+      </c>
+      <c r="B81" s="24" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="82" ht="15.75" customHeight="1">
+      <c r="A82" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="B82" s="24" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="77" ht="15.75" customHeight="1">
-      <c r="A77" s="24" t="s">
-        <v>235</v>
-      </c>
-      <c r="B77" s="24" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="78" ht="15.75" customHeight="1">
-      <c r="A78" s="24" t="s">
-        <v>237</v>
-      </c>
-      <c r="B78" s="24" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="79" ht="15.75" customHeight="1">
-      <c r="A79" s="24" t="s">
-        <v>239</v>
-      </c>
-      <c r="B79" s="24" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="80" ht="15.75" customHeight="1">
-      <c r="A80" s="24" t="s">
-        <v>240</v>
-      </c>
-      <c r="B80" s="24" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="81" ht="15.75" customHeight="1">
-      <c r="A81" s="24" t="s">
-        <v>242</v>
-      </c>
-      <c r="B81" s="24" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="82" ht="15.75" customHeight="1">
-      <c r="A82" s="24" t="s">
-        <v>244</v>
-      </c>
-      <c r="B82" s="24" t="s">
-        <v>232</v>
-      </c>
-    </row>
     <row r="83" ht="15.75" customHeight="1">
       <c r="A83" s="24" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B83" s="24" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="84" ht="15.75" customHeight="1">
       <c r="A84" s="24" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B84" s="24" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="85" ht="15.75" customHeight="1">
       <c r="A85" s="24" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B85" s="24" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="86" ht="15.75" customHeight="1">
       <c r="A86" s="24" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B86" s="24" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="87" ht="15.75" customHeight="1">
       <c r="A87" s="24" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="B87" s="24" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="88" ht="15.75" customHeight="1">
       <c r="A88" s="24" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B88" s="24" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="89" ht="15.75" customHeight="1">
       <c r="A89" s="24" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B89" s="24" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="90" ht="15.75" customHeight="1">
       <c r="A90" s="24" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="B90" s="24" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="91" ht="15.75" customHeight="1">
       <c r="A91" s="24" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="B91" s="24" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="92" ht="15.75" customHeight="1">
       <c r="A92" s="24" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B92" s="24" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="93" ht="15.75" customHeight="1">
       <c r="A93" s="24" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B93" s="24" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="94" ht="15.75" customHeight="1">
       <c r="A94" s="24" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B94" s="24" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="95" ht="15.75" customHeight="1">
       <c r="A95" s="24" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="B95" s="24" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="96" ht="15.75" customHeight="1">
       <c r="A96" s="24" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B96" s="24" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="97" ht="15.75" customHeight="1">
       <c r="A97" s="24" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B97" s="24" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="98" ht="15.75" customHeight="1">
       <c r="A98" s="24" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B98" s="24" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="99" ht="15.75" customHeight="1">
       <c r="A99" s="24" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B99" s="24" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="100" ht="15.75" customHeight="1">
       <c r="A100" s="24" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B100" s="24" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="101" ht="15.75" customHeight="1">
       <c r="A101" s="24" t="s">
+        <v>267</v>
+      </c>
+      <c r="B101" s="24" t="s">
         <v>265</v>
       </c>
-      <c r="B101" s="24" t="s">
-        <v>263</v>
-      </c>
     </row>
     <row r="102" ht="15.75" customHeight="1">
       <c r="A102" s="24" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B102" s="24" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="103" ht="15.75" customHeight="1">
       <c r="A103" s="24" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="B103" s="24" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="104" ht="15.75" customHeight="1">
       <c r="A104" s="24" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B104" s="24" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="105" ht="15.75" customHeight="1">
       <c r="A105" s="24" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B105" s="24" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="106" ht="15.75" customHeight="1">
       <c r="A106" s="24" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="B106" s="24" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="107" ht="15.75" customHeight="1">
       <c r="A107" s="24" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B107" s="24" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="108" ht="15.75" customHeight="1">
       <c r="A108" s="24" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="B108" s="24" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="109" ht="15.75" customHeight="1">
       <c r="A109" s="24" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="B109" s="24" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="110" ht="15.75" customHeight="1">
       <c r="A110" s="24" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B110" s="24" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="111" ht="15.75" customHeight="1">
       <c r="A111" s="24" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="B111" s="24" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="112" ht="15.75" customHeight="1"/>

</xml_diff>